<commit_message>
More fixes after testing the LED gauge and such
</commit_message>
<xml_diff>
--- a/LiPo Battery Gauge OpAmp Calcs.xlsx
+++ b/LiPo Battery Gauge OpAmp Calcs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Andrew\Google Drive\Electronics\52. Pride Badge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5766FD80-499F-44A3-B779-F1A76A3D868F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E0DA1B2-FDC6-4FE5-ACD3-96895BA12377}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13170" xr2:uid="{CDA544FD-AAAA-47D8-AEC1-BED803FC2C08}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -458,7 +459,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,20 +493,20 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2.42</v>
+        <v>1.95</v>
       </c>
       <c r="B2">
         <v>4.22</v>
       </c>
       <c r="C2">
-        <v>23200</v>
+        <v>27000</v>
       </c>
       <c r="D2">
-        <v>34800</v>
+        <v>30000</v>
       </c>
       <c r="E2">
         <f>B2-(B2/(C2+D2)*C2)</f>
-        <v>2.532</v>
+        <v>2.2210526315789472</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -539,18 +540,18 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>470</v>
+        <v>680</v>
       </c>
       <c r="B5">
         <f>A$2-(SUM(A$5:A5)/SUM(A$5:A$8)*A$2)</f>
-        <v>2.3146851851851853</v>
+        <v>1.8260747663551402</v>
       </c>
       <c r="D5">
         <v>4.2</v>
       </c>
       <c r="E5">
         <f>D5-(D5/(C$2+D$2)*C$2)</f>
-        <v>2.52</v>
+        <v>2.2105263157894739</v>
       </c>
       <c r="F5">
         <f>IF(D5&gt;=2, 1, 0)</f>
@@ -575,18 +576,18 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>470</v>
+        <v>680</v>
       </c>
       <c r="B6">
         <f>A$2-(SUM(A$5:A6)/SUM(A$5:A$8)*A$2)</f>
-        <v>2.2093703703703702</v>
+        <v>1.7021495327102802</v>
       </c>
       <c r="D6">
         <v>4.0999999999999996</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E22" si="0">D6-(D6/(C$2+D$2)*C$2)</f>
-        <v>2.46</v>
+        <v>2.1578947368421053</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F22" si="1">IF(D6&gt;=2, 1, 0)</f>
@@ -611,18 +612,18 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1200</v>
+        <v>680</v>
       </c>
       <c r="B7">
         <f>A$2-(SUM(A$5:A7)/SUM(A$5:A$8)*A$2)</f>
-        <v>1.9404814814814815</v>
+        <v>1.5782242990654205</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>2.4</v>
+        <v>2.1052631578947372</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
@@ -642,7 +643,7 @@
       </c>
       <c r="J7">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -658,7 +659,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2.34</v>
+        <v>2.0526315789473681</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
@@ -678,7 +679,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -690,7 +691,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>2.2799999999999998</v>
+        <v>1.9999999999999998</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
@@ -706,11 +707,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -719,7 +720,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>2.2199999999999998</v>
+        <v>1.9473684210526316</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
@@ -735,7 +736,7 @@
       </c>
       <c r="I10">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
@@ -748,7 +749,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2.16</v>
+        <v>1.8947368421052633</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
@@ -760,11 +761,11 @@
       </c>
       <c r="H11">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
@@ -777,7 +778,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>2.1</v>
+        <v>1.8421052631578947</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
@@ -789,11 +790,11 @@
       </c>
       <c r="H12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
@@ -806,7 +807,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>2.04</v>
+        <v>1.7894736842105263</v>
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
@@ -818,7 +819,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" si="4"/>
@@ -835,7 +836,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>1.98</v>
+        <v>1.7368421052631577</v>
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
@@ -847,7 +848,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="4"/>
@@ -864,7 +865,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1.9200000000000002</v>
+        <v>1.6842105263157896</v>
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
@@ -872,7 +873,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f t="shared" si="3"/>
@@ -893,7 +894,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.86</v>
+        <v>1.6315789473684212</v>
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
@@ -901,7 +902,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
@@ -922,7 +923,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>1.5789473684210527</v>
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
@@ -930,7 +931,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
@@ -951,7 +952,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1.74</v>
+        <v>1.5263157894736841</v>
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
@@ -980,7 +981,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1.68</v>
+        <v>1.4736842105263157</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
@@ -1009,7 +1010,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>1.62</v>
+        <v>1.4210526315789476</v>
       </c>
       <c r="F20">
         <f t="shared" si="1"/>
@@ -1038,7 +1039,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1.56</v>
+        <v>1.368421052631579</v>
       </c>
       <c r="F21">
         <f t="shared" si="1"/>
@@ -1067,7 +1068,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.3157894736842106</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>

</xml_diff>